<commit_message>
Update Bakery Sales Project
</commit_message>
<xml_diff>
--- a/Excel/Bakery Sales March 2020/Bakery Sales March 2020.xlsx
+++ b/Excel/Bakery Sales March 2020/Bakery Sales March 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/americamunoz/Desktop/Data Analyst Portfolio/Data-Analyst-Portfolio/Excel/Bakery Sales March 2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3089B05C-A6D7-1D4D-B019-B24ECC8F399D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20937CD-A3DB-7848-A745-D913AB44A233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15000" yWindow="3240" windowWidth="19900" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="12960" windowWidth="19900" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4570,8 +4570,8 @@
   </sheetPr>
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="89" workbookViewId="0">
-      <selection activeCell="R53" sqref="R53"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4966,8 +4966,8 @@
         <v>50</v>
       </c>
       <c r="I16" s="47">
-        <f>_xlfn.XLOOKUP(26,D2:D20,A2:A20,0)</f>
-        <v>0</v>
+        <f>_xlfn.XLOOKUP(H16,D2:D20,A2:A20)</f>
+        <v>45016</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16">
@@ -5016,8 +5016,8 @@
         <v>80</v>
       </c>
       <c r="I18" s="47">
-        <f>_xlfn.XLOOKUP(41,D4:D22,A4:A22,0)</f>
-        <v>0</v>
+        <f>_xlfn.XLOOKUP(H18,D4:D22,A4:A22)</f>
+        <v>45016</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16">

</xml_diff>